<commit_message>
Update in User registration
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC23_Verify_UserRegistration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\Kaman_ECTEST_IE_Support\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8BA91A-AD65-42E0-A91E-5C472055D9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7474F7F6-56DD-42DE-A24C-2EC86D052D18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
   <si>
     <t>TestCase</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>CLICK_PRE_ENTERTEXT</t>
   </si>
 </sst>
 </file>
@@ -563,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -645,8 +648,8 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
+      <c r="B6" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>16</v>
@@ -654,9 +657,7 @@
       <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
@@ -664,101 +665,103 @@
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
+      <c r="B10" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3"/>
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -767,10 +770,10 @@
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="5" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>37</v>
@@ -779,20 +782,26 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>37</v>
@@ -801,12 +810,18 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
@@ -814,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>37</v>
@@ -824,17 +839,11 @@
     <row r="20" spans="1:5">
       <c r="A20" s="3"/>
       <c r="B20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
@@ -842,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>37</v>
@@ -864,12 +873,84 @@
         <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3"/>
+      <c r="B24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3"/>
+      <c r="B25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3"/>
+      <c r="B26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3"/>
+      <c r="B27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3"/>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>